<commit_message>
stops resized to picbox
</commit_message>
<xml_diff>
--- a/SchemaBusy/bin/Debug/Lokace zastávek.xlsx
+++ b/SchemaBusy/bin/Debug/Lokace zastávek.xlsx
@@ -12,11 +12,12 @@
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Jméno zastávky</t>
   </si>
@@ -109,6 +110,42 @@
   </si>
   <si>
     <t>Uherské Hradiště,Sady,rozc.</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Sady</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Sady,Za Kovárnou</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Vésky,hor.konec</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Vésky,střed</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Míkovice,Hlavní</t>
+  </si>
+  <si>
+    <t>Kunovice,,koupaliště</t>
+  </si>
+  <si>
+    <t>Kunovice,,Lidická</t>
+  </si>
+  <si>
+    <t>Kunovice,,Na Rynku</t>
+  </si>
+  <si>
+    <t>Kunovice,,rozc.k žel.st.0.5</t>
+  </si>
+  <si>
+    <t>Kunovice,,Na Bělince</t>
+  </si>
+  <si>
+    <t>Kunovice,,Panská</t>
+  </si>
+  <si>
+    <t>Kunovice,,Let</t>
   </si>
 </sst>
 </file>
@@ -145,11 +182,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -453,14 +487,14 @@
   <dimension ref="B1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="2" customWidth="1"/>
     <col min="10" max="10" width="3.5703125" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
@@ -475,10 +509,10 @@
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" t="s">
@@ -501,11 +535,11 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <f xml:space="preserve"> B2 * $K$2</f>
         <v>527.75</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <f xml:space="preserve"> C2 * $K$2</f>
         <v>290.375</v>
       </c>
@@ -530,11 +564,11 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E43" si="0" xml:space="preserve"> B3 * $K$2</f>
         <v>430.125</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f t="shared" ref="F3:F43" si="1" xml:space="preserve"> C3 * $K$2</f>
         <v>190.625</v>
       </c>
@@ -546,14 +580,14 @@
       <c r="C4">
         <v>2622</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>366.375</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f t="shared" si="1"/>
         <v>327.75</v>
       </c>
@@ -565,14 +599,14 @@
       <c r="C5">
         <v>1996</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>665.875</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f t="shared" si="1"/>
         <v>249.5</v>
       </c>
@@ -584,14 +618,14 @@
       <c r="C6">
         <v>1486</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>705.625</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f t="shared" si="1"/>
         <v>185.75</v>
       </c>
@@ -603,14 +637,14 @@
       <c r="C7">
         <v>971</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>746.5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f t="shared" si="1"/>
         <v>121.375</v>
       </c>
@@ -622,14 +656,14 @@
       <c r="C8">
         <v>472</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>811.75</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
@@ -641,14 +675,14 @@
       <c r="C9">
         <v>621</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>869.125</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <f t="shared" si="1"/>
         <v>77.625</v>
       </c>
@@ -660,14 +694,14 @@
       <c r="C10">
         <v>476</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>851.625</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <f t="shared" si="1"/>
         <v>59.5</v>
       </c>
@@ -679,14 +713,14 @@
       <c r="C11">
         <v>122</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>902.375</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <f t="shared" si="1"/>
         <v>15.25</v>
       </c>
@@ -698,14 +732,14 @@
       <c r="C12">
         <v>2946</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>539.25</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <f t="shared" si="1"/>
         <v>368.25</v>
       </c>
@@ -717,14 +751,14 @@
       <c r="C13">
         <v>3548</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f xml:space="preserve"> B13 * $K$2</f>
         <v>541.375</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f xml:space="preserve"> C13 * $K$2</f>
         <v>443.5</v>
       </c>
@@ -736,14 +770,14 @@
       <c r="C14">
         <v>3771</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>551.5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f t="shared" si="1"/>
         <v>471.375</v>
       </c>
@@ -755,14 +789,14 @@
       <c r="C15">
         <v>3448</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>649.625</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <f t="shared" si="1"/>
         <v>431</v>
       </c>
@@ -774,14 +808,14 @@
       <c r="C16">
         <v>3695</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>653.875</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
         <v>461.875</v>
       </c>
@@ -793,14 +827,14 @@
       <c r="C17">
         <v>3523</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>699.625</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <f t="shared" si="1"/>
         <v>440.375</v>
       </c>
@@ -812,14 +846,14 @@
       <c r="C18">
         <v>3235</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>687.75</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <f t="shared" si="1"/>
         <v>404.375</v>
       </c>
@@ -831,14 +865,14 @@
       <c r="C19">
         <v>3032</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>725.25</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <f t="shared" si="1"/>
         <v>379</v>
       </c>
@@ -850,14 +884,14 @@
       <c r="C20">
         <v>2954</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>743.5</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <f t="shared" si="1"/>
         <v>369.25</v>
       </c>
@@ -869,15 +903,15 @@
       <c r="C21">
         <v>2723</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="2">
-        <f>B21 * $K$2</f>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
         <v>541.25</v>
       </c>
-      <c r="F21" s="2">
-        <f>C21 * $K$2</f>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
         <v>340.375</v>
       </c>
     </row>
@@ -888,14 +922,14 @@
       <c r="C22">
         <v>2910</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>672.5</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <f t="shared" si="1"/>
         <v>363.75</v>
       </c>
@@ -907,14 +941,14 @@
       <c r="C23">
         <v>2576</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>638.125</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <f t="shared" si="1"/>
         <v>322</v>
       </c>
@@ -926,204 +960,312 @@
       <c r="C24">
         <v>3842</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>559.75</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <f t="shared" si="1"/>
         <v>480.25</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B25">
+        <v>5253</v>
+      </c>
+      <c r="C25">
+        <v>4298</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>656.625</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>537.25</v>
       </c>
     </row>
     <row r="26" spans="2:6">
-      <c r="E26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B26">
+        <v>5691</v>
+      </c>
+      <c r="C26">
+        <v>4452</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>711.375</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>556.5</v>
       </c>
     </row>
     <row r="27" spans="2:6">
-      <c r="E27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B27">
+        <v>6575</v>
+      </c>
+      <c r="C27">
+        <v>4799</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>821.875</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>599.875</v>
       </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="E28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B28">
+        <v>6778</v>
+      </c>
+      <c r="C28">
+        <v>5215</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>847.25</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>651.875</v>
       </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="E29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B29">
+        <v>7097</v>
+      </c>
+      <c r="C29">
+        <v>5875</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>887.125</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>734.375</v>
       </c>
     </row>
     <row r="30" spans="2:6">
-      <c r="E30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B30">
+        <v>6172</v>
+      </c>
+      <c r="C30">
+        <v>5809</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>771.5</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>726.125</v>
       </c>
     </row>
     <row r="31" spans="2:6">
-      <c r="E31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B31">
+        <v>4703</v>
+      </c>
+      <c r="C31">
+        <v>5550</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>587.875</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>693.75</v>
       </c>
     </row>
     <row r="32" spans="2:6">
-      <c r="E32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
-      <c r="E33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
-      <c r="E34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
-      <c r="E35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
-      <c r="E36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
-      <c r="E37" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6">
-      <c r="E38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6">
-      <c r="E39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6">
-      <c r="E40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6">
-      <c r="E41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
-      <c r="E42" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6">
-      <c r="E43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="2">
+      <c r="B32">
+        <v>4362</v>
+      </c>
+      <c r="C32">
+        <v>5260</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>545.25</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>657.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33">
+        <v>4334</v>
+      </c>
+      <c r="C33">
+        <v>4439</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>541.75</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>554.875</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34">
+        <v>4041</v>
+      </c>
+      <c r="C34">
+        <v>5412</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>505.125</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="1"/>
+        <v>676.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35">
+        <v>3488</v>
+      </c>
+      <c r="C35">
+        <v>5181</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="0"/>
+        <v>436</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="1"/>
+        <v>647.625</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36">
+        <v>2137</v>
+      </c>
+      <c r="C36">
+        <v>4915</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="0"/>
+        <v>267.125</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="1"/>
+        <v>614.375</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="E38" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="E39" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="E40" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="E41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="E42" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="E43" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
stops can have names
</commit_message>
<xml_diff>
--- a/SchemaBusy/bin/Debug/Lokace zastávek.xlsx
+++ b/SchemaBusy/bin/Debug/Lokace zastávek.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Jméno zastávky</t>
   </si>
@@ -146,6 +146,30 @@
   </si>
   <si>
     <t>Kunovice,,Let</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,,Jiřího z Poděbrad</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,,Svatojiřské nábřeží</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,,Stará Tenice</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,,žel.st.</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,,Purkyňova</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,,nemocnice</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Štěpnice,Zahrádky</t>
+  </si>
+  <si>
+    <t>Uherské Hradiště,Štěpnice,U Olšávky</t>
   </si>
 </sst>
 </file>
@@ -484,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M43"/>
+  <dimension ref="B1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,7 +589,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E43" si="0" xml:space="preserve"> B3 * $K$2</f>
+        <f t="shared" ref="E3:F43" si="0" xml:space="preserve"> B3 * $K$2</f>
         <v>430.125</v>
       </c>
       <c r="F3" s="1">
@@ -1201,72 +1225,434 @@
       </c>
     </row>
     <row r="37" spans="2:6">
+      <c r="B37">
+        <v>4097</v>
+      </c>
+      <c r="C37">
+        <v>2758</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>512.125</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>344.75</v>
       </c>
     </row>
     <row r="38" spans="2:6">
+      <c r="B38">
+        <v>3628</v>
+      </c>
+      <c r="C38">
+        <v>2038</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>453.5</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>254.75</v>
       </c>
     </row>
     <row r="39" spans="2:6">
+      <c r="B39">
+        <v>3303</v>
+      </c>
+      <c r="C39">
+        <v>2263</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>412.875</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>282.875</v>
       </c>
     </row>
     <row r="40" spans="2:6">
+      <c r="B40">
+        <v>3734</v>
+      </c>
+      <c r="C40">
+        <v>2631</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>466.75</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>328.875</v>
       </c>
     </row>
     <row r="41" spans="2:6">
+      <c r="B41">
+        <v>3475</v>
+      </c>
+      <c r="C41">
+        <v>2893</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>434.375</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>361.625</v>
       </c>
     </row>
     <row r="42" spans="2:6">
+      <c r="B42">
+        <v>3334</v>
+      </c>
+      <c r="C42">
+        <v>2948</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>416.75</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>368.5</v>
       </c>
     </row>
     <row r="43" spans="2:6">
+      <c r="B43">
+        <v>2697</v>
+      </c>
+      <c r="C43">
+        <v>2732</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E43" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E43:E72" si="2" xml:space="preserve"> B43 * $K$2</f>
+        <v>337.125</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F43:F72" si="3" xml:space="preserve"> C43 * $K$2</f>
+        <v>341.5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44">
+        <v>3785</v>
+      </c>
+      <c r="C44">
+        <v>2798</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="2"/>
+        <v>473.125</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>349.75</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="E45" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="E46" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="E47" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="E48" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6">
+      <c r="E49" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6">
+      <c r="E50" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6">
+      <c r="E51" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6">
+      <c r="E52" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6">
+      <c r="E53" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6">
+      <c r="E54" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6">
+      <c r="E55" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="5:6">
+      <c r="E56" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="5:6">
+      <c r="E57" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="5:6">
+      <c r="E58" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="5:6">
+      <c r="E59" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:6">
+      <c r="E60" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="5:6">
+      <c r="E61" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="5:6">
+      <c r="E62" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="5:6">
+      <c r="E63" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="5:6">
+      <c r="E64" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6">
+      <c r="E65" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6">
+      <c r="E66" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6">
+      <c r="E67" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="5:6">
+      <c r="E68" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="5:6">
+      <c r="E69" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="5:6">
+      <c r="E70" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="5:6">
+      <c r="E71" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="5:6">
+      <c r="E72" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>